<commit_message>
Correccion ejercicio clase 11
</commit_message>
<xml_diff>
--- a/Clase_11_Maquinas_Virtuales/Ejercicio de algoritmos de planificación - Práctica.xlsx
+++ b/Clase_11_Maquinas_Virtuales/Ejercicio de algoritmos de planificación - Práctica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LOBO\Desktop\DH\II\C11A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46FAC84-6AB8-43B9-A906-9E5DD31DD2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5103651A-9B42-4AA3-B62F-0A557F8747AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIFO" sheetId="1" r:id="rId1"/>
@@ -1220,7 +1220,7 @@
   <dimension ref="A1:CI34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:L15"/>
+      <selection activeCell="AK29" sqref="AK29:BB31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2664,7 +2664,7 @@
   <dimension ref="A1:BD1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="A12:XFD34"/>
+      <selection activeCell="AN39" sqref="AN39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24758,7 +24758,7 @@
   <dimension ref="A1:BD34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD34"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25691,7 +25691,7 @@
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="26"/>
+      <c r="G25" s="16"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
       <c r="J25" s="26"/>
@@ -25700,14 +25700,14 @@
       <c r="M25" s="26"/>
       <c r="N25" s="26"/>
       <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
+      <c r="P25" s="16"/>
       <c r="Q25" s="26"/>
       <c r="R25" s="26"/>
       <c r="S25" s="26"/>
       <c r="T25" s="26"/>
       <c r="U25" s="26"/>
       <c r="V25" s="26"/>
-      <c r="W25" s="16"/>
+      <c r="W25" s="26"/>
       <c r="X25" s="26"/>
       <c r="Y25" s="26"/>
       <c r="Z25" s="26"/>
@@ -25715,7 +25715,7 @@
       <c r="AB25" s="26"/>
       <c r="AC25" s="26"/>
       <c r="AD25" s="26"/>
-      <c r="AE25" s="16"/>
+      <c r="AE25" s="26"/>
       <c r="AF25" s="26"/>
       <c r="AG25" s="26"/>
       <c r="AH25" s="26"/>
@@ -25748,25 +25748,25 @@
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="26"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="17"/>
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
       <c r="K26" s="26"/>
       <c r="L26" s="26"/>
       <c r="M26" s="26"/>
       <c r="N26" s="26"/>
-      <c r="O26" s="17"/>
+      <c r="O26" s="26"/>
       <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
+      <c r="Q26" s="17"/>
       <c r="R26" s="26"/>
       <c r="S26" s="26"/>
       <c r="T26" s="26"/>
       <c r="U26" s="26"/>
       <c r="V26" s="26"/>
       <c r="W26" s="26"/>
-      <c r="X26" s="17"/>
-      <c r="Y26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="17"/>
       <c r="Z26" s="26"/>
       <c r="AA26" s="26"/>
       <c r="AB26" s="26"/>
@@ -25808,25 +25808,25 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="18"/>
       <c r="L27" s="26"/>
       <c r="M27" s="26"/>
       <c r="N27" s="26"/>
       <c r="O27" s="26"/>
       <c r="P27" s="26"/>
       <c r="Q27" s="26"/>
-      <c r="R27" s="18"/>
+      <c r="R27" s="26"/>
       <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
+      <c r="T27" s="18"/>
       <c r="U27" s="26"/>
       <c r="V27" s="26"/>
       <c r="W27" s="26"/>
       <c r="X27" s="26"/>
       <c r="Y27" s="26"/>
       <c r="Z27" s="26"/>
-      <c r="AA27" s="18"/>
-      <c r="AB27" s="26"/>
+      <c r="AA27" s="26"/>
+      <c r="AB27" s="18"/>
       <c r="AC27" s="26"/>
       <c r="AD27" s="26"/>
       <c r="AE27" s="26"/>
@@ -25867,25 +25867,25 @@
       <c r="I28" s="26"/>
       <c r="J28" s="26"/>
       <c r="K28" s="26"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="19"/>
       <c r="N28" s="26"/>
       <c r="O28" s="26"/>
       <c r="P28" s="26"/>
       <c r="Q28" s="26"/>
       <c r="R28" s="26"/>
       <c r="S28" s="26"/>
-      <c r="T28" s="19"/>
+      <c r="T28" s="26"/>
       <c r="U28" s="26"/>
-      <c r="V28" s="26"/>
+      <c r="V28" s="19"/>
       <c r="W28" s="26"/>
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
       <c r="Z28" s="26"/>
       <c r="AA28" s="26"/>
       <c r="AB28" s="26"/>
-      <c r="AC28" s="19"/>
-      <c r="AD28" s="26"/>
+      <c r="AC28" s="26"/>
+      <c r="AD28" s="19"/>
       <c r="AE28" s="26"/>
       <c r="AF28" s="26"/>
       <c r="AG28" s="26"/>
@@ -25926,17 +25926,17 @@
       <c r="K29" s="26"/>
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="20"/>
       <c r="P29" s="26"/>
       <c r="Q29" s="26"/>
       <c r="R29" s="26"/>
       <c r="S29" s="26"/>
       <c r="T29" s="26"/>
       <c r="U29" s="26"/>
-      <c r="V29" s="20"/>
+      <c r="V29" s="26"/>
       <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
+      <c r="X29" s="20"/>
       <c r="Y29" s="26"/>
       <c r="Z29" s="26"/>
       <c r="AA29" s="26"/>
@@ -25980,25 +25980,25 @@
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
       <c r="J30" s="26"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="21"/>
       <c r="M30" s="26"/>
       <c r="N30" s="26"/>
       <c r="O30" s="26"/>
       <c r="P30" s="26"/>
       <c r="Q30" s="26"/>
       <c r="R30" s="26"/>
-      <c r="S30" s="21"/>
+      <c r="S30" s="26"/>
       <c r="T30" s="26"/>
-      <c r="U30" s="26"/>
+      <c r="U30" s="21"/>
       <c r="V30" s="26"/>
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
       <c r="Y30" s="26"/>
       <c r="Z30" s="26"/>
       <c r="AA30" s="26"/>
-      <c r="AB30" s="21"/>
-      <c r="AC30" s="26"/>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="21"/>
       <c r="AD30" s="26"/>
       <c r="AE30" s="26"/>
       <c r="AF30" s="26"/>
@@ -26035,25 +26035,25 @@
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="22"/>
       <c r="K31" s="26"/>
       <c r="L31" s="26"/>
       <c r="M31" s="26"/>
       <c r="N31" s="26"/>
       <c r="O31" s="26"/>
       <c r="P31" s="26"/>
-      <c r="Q31" s="22"/>
+      <c r="Q31" s="26"/>
       <c r="R31" s="26"/>
-      <c r="S31" s="26"/>
+      <c r="S31" s="22"/>
       <c r="T31" s="26"/>
       <c r="U31" s="26"/>
       <c r="V31" s="26"/>
       <c r="W31" s="26"/>
       <c r="X31" s="26"/>
       <c r="Y31" s="26"/>
-      <c r="Z31" s="22"/>
-      <c r="AA31" s="26"/>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="22"/>
       <c r="AB31" s="26"/>
       <c r="AC31" s="26"/>
       <c r="AD31" s="26"/>
@@ -26096,25 +26096,25 @@
       <c r="J32" s="26"/>
       <c r="K32" s="26"/>
       <c r="L32" s="26"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="23"/>
       <c r="O32" s="26"/>
       <c r="P32" s="26"/>
       <c r="Q32" s="26"/>
       <c r="R32" s="26"/>
       <c r="S32" s="26"/>
       <c r="T32" s="26"/>
-      <c r="U32" s="23"/>
+      <c r="U32" s="26"/>
       <c r="V32" s="26"/>
-      <c r="W32" s="26"/>
+      <c r="W32" s="23"/>
       <c r="X32" s="26"/>
       <c r="Y32" s="26"/>
       <c r="Z32" s="26"/>
       <c r="AA32" s="26"/>
       <c r="AB32" s="26"/>
       <c r="AC32" s="26"/>
-      <c r="AD32" s="23"/>
-      <c r="AE32" s="26"/>
+      <c r="AD32" s="26"/>
+      <c r="AE32" s="23"/>
       <c r="AF32" s="26"/>
       <c r="AG32" s="26"/>
       <c r="AH32" s="26"/>
@@ -26148,25 +26148,25 @@
       <c r="E33" s="26"/>
       <c r="F33" s="26"/>
       <c r="G33" s="26"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="24"/>
       <c r="J33" s="26"/>
       <c r="K33" s="26"/>
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
       <c r="N33" s="26"/>
       <c r="O33" s="26"/>
-      <c r="P33" s="24"/>
+      <c r="P33" s="26"/>
       <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
+      <c r="R33" s="24"/>
       <c r="S33" s="26"/>
       <c r="T33" s="26"/>
       <c r="U33" s="26"/>
       <c r="V33" s="26"/>
       <c r="W33" s="26"/>
       <c r="X33" s="26"/>
-      <c r="Y33" s="24"/>
-      <c r="Z33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="24"/>
       <c r="AA33" s="26"/>
       <c r="AB33" s="26"/>
       <c r="AC33" s="26"/>
@@ -26368,8 +26368,8 @@
   </sheetPr>
   <dimension ref="A1:AW34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA12" sqref="A12:XFD34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y40" sqref="Y40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31487,7 +31487,7 @@
   </sheetPr>
   <dimension ref="A1:EH1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AJ8" sqref="AJ8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
arreglos ejercicio clase 11
</commit_message>
<xml_diff>
--- a/Clase_11_Maquinas_Virtuales/Ejercicio de algoritmos de planificación - Práctica.xlsx
+++ b/Clase_11_Maquinas_Virtuales/Ejercicio de algoritmos de planificación - Práctica.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="6"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FIFO" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
     <col min="70" max="70" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +519,7 @@
       <c r="AR1" s="23"/>
       <c r="AS1" s="23"/>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -572,7 +572,7 @@
       <c r="AR2" s="23"/>
       <c r="AS2" s="23"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -625,7 +625,7 @@
       <c r="AR3" s="23"/>
       <c r="AS3" s="23"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -678,7 +678,7 @@
       <c r="AR4" s="23"/>
       <c r="AS4" s="23"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -731,7 +731,7 @@
       <c r="AR5" s="23"/>
       <c r="AS5" s="23"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="AR6" s="23"/>
       <c r="AS6" s="23"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -837,7 +837,7 @@
       <c r="AR7" s="23"/>
       <c r="AS7" s="23"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -890,7 +890,7 @@
       <c r="AR8" s="23"/>
       <c r="AS8" s="23"/>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -943,7 +943,7 @@
       <c r="AR9" s="23"/>
       <c r="AS9" s="23"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -1040,7 +1040,7 @@
       <c r="AR11" s="23"/>
       <c r="AS11" s="23"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="AR12" s="23"/>
       <c r="AS12" s="23"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
     </row>
-    <row r="17" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C17" s="7" t="s">
         <v>7</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="AB51" s="1" t="s">
         <v>0</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="AB52" s="2" t="s">
         <v>3</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="AB53" s="4" t="s">
         <v>4</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
         <v>3</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C56" s="4" t="s">
         <v>4</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C57" s="5" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C58" s="6" t="s">
         <v>6</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="7" t="s">
         <v>7</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="8" t="s">
         <v>8</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="9" t="s">
         <v>9</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="O61" s="9"/>
       <c r="P61" s="9"/>
     </row>
-    <row r="62" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="10" t="s">
         <v>10</v>
       </c>
@@ -1741,14 +1741,14 @@
       <c r="M62" s="10"/>
       <c r="N62" s="10"/>
     </row>
-    <row r="63" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="11" t="s">
         <v>11</v>
       </c>
       <c r="P63" s="11"/>
       <c r="Q63" s="11"/>
     </row>
-    <row r="64" spans="3:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D64" s="20">
         <v>0</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="4:54" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:54" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="4"/>
@@ -23347,8 +23347,8 @@
   </sheetPr>
   <dimension ref="A1:CH1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BL31" sqref="BL31:CH31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18:U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23973,26 +23973,19 @@
       <c r="E25" s="28"/>
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
       <c r="O25" s="23"/>
       <c r="P25" s="23"/>
       <c r="Q25" s="23"/>
       <c r="R25" s="23"/>
       <c r="S25" s="23"/>
       <c r="T25" s="23"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
     </row>
     <row r="26" spans="3:86" x14ac:dyDescent="0.2">
       <c r="C26" s="5" t="s">
@@ -24002,17 +23995,13 @@
       <c r="E26" s="28"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
       <c r="L26" s="23"/>
       <c r="M26" s="23"/>
       <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
       <c r="S26" s="23"/>
       <c r="T26" s="23"/>
       <c r="U26" s="23"/>
@@ -24039,18 +24028,13 @@
       <c r="M27" s="23"/>
       <c r="N27" s="23"/>
       <c r="O27" s="23"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
       <c r="U27" s="23"/>
       <c r="V27" s="23"/>
-      <c r="W27" s="23"/>
-      <c r="X27" s="23"/>
-      <c r="Y27" s="23"/>
-      <c r="Z27" s="23"/>
-      <c r="AA27" s="23"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
     </row>
     <row r="28" spans="3:86" x14ac:dyDescent="0.2">
       <c r="C28" s="7" t="s">
@@ -24139,17 +24123,13 @@
       <c r="I30" s="23"/>
       <c r="J30" s="23"/>
       <c r="K30" s="23"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
       <c r="P30" s="23"/>
       <c r="Q30" s="23"/>
       <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
       <c r="W30" s="23"/>
       <c r="X30" s="23"/>
       <c r="Y30" s="23"/>
@@ -27325,7 +27305,7 @@
   <dimension ref="A1:BN35"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="BD29" sqref="BD29"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27336,12 +27316,12 @@
     <col min="4" max="54" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -27352,7 +27332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -27363,7 +27343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -27374,7 +27354,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -27385,7 +27365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -27396,7 +27376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -27407,7 +27387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
@@ -27418,7 +27398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -27429,7 +27409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -27440,7 +27420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>11</v>
       </c>
@@ -27754,13 +27734,15 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="27"/>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="3:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="27"/>
       <c r="J27" s="4"/>
       <c r="M27" s="4"/>
       <c r="Q27" s="4"/>
@@ -27835,7 +27817,8 @@
       <c r="C34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="27"/>
       <c r="L34" s="11"/>
       <c r="P34" s="11"/>
       <c r="U34" s="11"/>
@@ -28060,7 +28043,7 @@
     <col min="4" max="42" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -28071,7 +28054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -28082,7 +28065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -28093,7 +28076,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -28104,7 +28087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -28115,7 +28098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -28126,7 +28109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -28137,7 +28120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -28148,7 +28131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -28159,7 +28142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -28765,7 +28748,7 @@
     <col min="4" max="42" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -28776,7 +28759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -28787,7 +28770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -28798,7 +28781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -28809,7 +28792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -28820,7 +28803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -28831,7 +28814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -28842,7 +28825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -28853,7 +28836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -28864,7 +28847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -29493,7 +29476,7 @@
   </sheetPr>
   <dimension ref="A1:EZ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="EX32" sqref="EX32:EZ32"/>
     </sheetView>
   </sheetViews>
@@ -29503,7 +29486,7 @@
     <col min="4" max="42" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -29514,7 +29497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -29525,7 +29508,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -29536,7 +29519,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -29547,7 +29530,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -29558,7 +29541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -29569,7 +29552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -29580,7 +29563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -29591,7 +29574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -29602,7 +29585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>

</xml_diff>